<commit_message>
shading + genome traits
</commit_message>
<xml_diff>
--- a/genomic_traits/trait_gene_annotations/N related  enzymes.xlsx
+++ b/genomic_traits/trait_gene_annotations/N related  enzymes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\genomic_traits\trait_gene_annotations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA52D182-956F-4013-9E36-4E4EC223DAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D8455-BE29-401C-901C-8CF35026780E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{2BE49138-A04E-4DD4-94E0-C7AA9414B3B9}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>D-/L-Amino acid oxidases</t>
   </si>
   <si>
-    <t>3.6.3</t>
-  </si>
-  <si>
     <t>3.6.3.21</t>
   </si>
   <si>
@@ -534,6 +531,9 @@
   </si>
   <si>
     <t>Other enzymes relevant to N cycling</t>
+  </si>
+  <si>
+    <t>3.6.3.x</t>
   </si>
 </sst>
 </file>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427B33E7-BDCA-4CC0-B7C6-F4E6A93D8B96}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:A79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -928,10 +928,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -939,324 +939,324 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
         <v>96</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
         <v>101</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
         <v>104</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>5</v>
@@ -1278,286 +1278,286 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
         <v>111</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
         <v>113</v>
-      </c>
-      <c r="C32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1565,10 +1565,10 @@
         <v>16</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1576,10 +1576,10 @@
         <v>16</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1587,10 +1587,10 @@
         <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1598,10 +1598,10 @@
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1609,10 +1609,10 @@
         <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1620,10 +1620,10 @@
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1631,10 +1631,10 @@
         <v>16</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1642,10 +1642,10 @@
         <v>16</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1653,10 +1653,10 @@
         <v>16</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1664,10 +1664,10 @@
         <v>16</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1675,10 +1675,10 @@
         <v>16</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1686,10 +1686,10 @@
         <v>16</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1697,10 +1697,10 @@
         <v>16</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1716,7 +1716,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>10</v>
@@ -1727,115 +1727,115 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" t="s">
         <v>148</v>
-      </c>
-      <c r="C69" t="s">
-        <v>79</v>
-      </c>
-      <c r="D69" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>13</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>14</v>

</xml_diff>